<commit_message>
Learning by not doing regressions
</commit_message>
<xml_diff>
--- a/Tables/SS_learning.xlsx
+++ b/Tables/SS_learning.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CACF87-8992-4C25-8A93-124EBBEDC1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25950" yWindow="-5850" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25950" yWindow="-5850" windowWidth="21600" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="SS_learning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -219,55 +219,55 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -586,21 +586,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:AU27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.7265625" style="11" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="10.6328125" style="11" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="10.7265625" style="11" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="11.54296875" style="11" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="15" t="s">
@@ -610,115 +610,115 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="L5">
-        <v>8.1632653061224483E-2</v>
+        <v>0.068181818181818177</v>
       </c>
       <c r="M5">
-        <v>6.25E-2</v>
+        <v>0.072463768115942032</v>
       </c>
       <c r="N5">
-        <v>4.1666666666666664E-2</v>
+        <v>0.056603773584905662</v>
       </c>
       <c r="O5">
-        <v>0.3235294117647059</v>
+        <v>0.34782608695652173</v>
       </c>
       <c r="P5">
-        <v>6.1224489795918366E-2</v>
+        <v>0.066666666666666666</v>
       </c>
       <c r="Q5">
-        <v>6.8965517241379309E-2</v>
+        <v>0.07407407407407407</v>
       </c>
       <c r="R5">
-        <v>1.680672268907563E-2</v>
+        <v>0.030303030303030304</v>
       </c>
       <c r="S5">
-        <v>0.13636363636363635</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="T5">
-        <v>0.63318773791485183</v>
+        <v>0.91138131955600066</v>
       </c>
       <c r="U5">
-        <v>0.38398587751942559</v>
+        <v>0.82461769586545186</v>
       </c>
       <c r="V5">
-        <v>1.4732288002943204E-2</v>
+        <v>0.013564805283350202</v>
       </c>
       <c r="W5">
-        <v>0.70682530916285047</v>
+        <v>0.97808876311225568</v>
       </c>
       <c r="X5">
-        <v>0.83973491549943147</v>
+        <v>0.92740043644858183</v>
       </c>
       <c r="Y5">
-        <v>0.13435550270331939</v>
+        <v>0.40634140811298913</v>
       </c>
       <c r="Z5">
-        <v>0.53221411897800386</v>
+        <v>0.21188197171210843</v>
       </c>
       <c r="AA5">
-        <v>0.48369701379892016</v>
+        <v>0.6949887776671434</v>
       </c>
       <c r="AB5">
-        <v>7.4363074905941838E-3</v>
+        <v>0.01703624221488393</v>
       </c>
       <c r="AC5">
-        <v>0.97360733147127931</v>
+        <v>0.89351820741680366</v>
       </c>
       <c r="AD5">
-        <v>0.90864075202982297</v>
+        <v>0.97916676003465897</v>
       </c>
       <c r="AE5">
-        <v>0.11438569646077601</v>
+        <v>0.25706829366071565</v>
       </c>
       <c r="AF5">
-        <v>0.36395968706087789</v>
+        <v>0.20872389344789977</v>
       </c>
       <c r="AG5">
-        <v>1.7955343033889285E-3</v>
+        <v>0.011734441106661891</v>
       </c>
       <c r="AH5">
-        <v>0.56747949381615415</v>
+        <v>0.80849018563525132</v>
       </c>
       <c r="AI5">
-        <v>0.59415754778454</v>
+        <v>0.7723732627494021</v>
       </c>
       <c r="AJ5">
-        <v>0.29672941706053563</v>
+        <v>0.50052526360916905</v>
       </c>
       <c r="AK5">
-        <v>0.22906329495436681</v>
+        <v>0.16765757855540159</v>
       </c>
       <c r="AL5">
-        <v>4.9727697227380102E-3</v>
+        <v>0.0097748789346420884</v>
       </c>
       <c r="AM5">
-        <v>1.1563449391979322E-2</v>
+        <v>0.019449537871593373</v>
       </c>
       <c r="AN5">
-        <v>5.3003999562476129E-4</v>
+        <v>0.0021294895512379841</v>
       </c>
       <c r="AO5">
-        <v>3.7037466444741138E-2</v>
+        <v>0.33038778340145369</v>
       </c>
       <c r="AP5">
-        <v>0.89692949316409243</v>
+        <v>0.90850331591224687</v>
       </c>
       <c r="AQ5">
-        <v>0.22432349271784366</v>
+        <v>0.3989092965964347</v>
       </c>
       <c r="AR5">
-        <v>0.30800858556578653</v>
+        <v>0.16780273381579652</v>
       </c>
       <c r="AS5">
-        <v>0.28608230872881052</v>
+        <v>0.43105846353394817</v>
       </c>
       <c r="AT5">
-        <v>0.44786898802008868</v>
+        <v>0.24135638719487112</v>
       </c>
       <c r="AU5">
-        <v>0.10151353216512879</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.087143941038846401</v>
+      </c>
+    </row>
+    <row r="6" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="5"/>
       <c r="C6" s="10" t="s">
@@ -734,31 +734,59 @@
         <v>3</v>
       </c>
       <c r="L6">
-        <v>4.1137262589909962E-2</v>
+        <v>0.039704245002748807</v>
       </c>
       <c r="M6">
-        <v>2.6375081929891908E-2</v>
+        <v>0.030681682420916231</v>
       </c>
       <c r="N6">
-        <v>2.0661807416692036E-2</v>
+        <v>0.033153944802459187</v>
       </c>
       <c r="O6">
-        <v>8.6408942996498664E-2</v>
+        <v>0.10218620161789856</v>
       </c>
       <c r="P6">
-        <v>3.3633491231636094E-2</v>
+        <v>0.036357553079168957</v>
       </c>
       <c r="Q6">
-        <v>4.7480252893206787E-2</v>
+        <v>0.051016228790772493</v>
       </c>
       <c r="R6">
-        <v>1.2086762151894734E-2</v>
+        <v>0.021609825968389312</v>
       </c>
       <c r="S6">
-        <v>7.6135585316286641E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+        <v>0.12483537131240699</v>
+      </c>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6"/>
+      <c r="AL6"/>
+      <c r="AM6"/>
+      <c r="AN6"/>
+      <c r="AO6"/>
+      <c r="AP6"/>
+      <c r="AQ6"/>
+      <c r="AR6"/>
+      <c r="AS6"/>
+      <c r="AT6"/>
+      <c r="AU6"/>
+    </row>
+    <row r="7" ht="15" customHeight="true" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>0</v>
       </c>
@@ -782,31 +810,59 @@
         <v>0.32400000000000001</v>
       </c>
       <c r="L7">
-        <v>271</v>
+        <v>86</v>
       </c>
       <c r="M7">
-        <v>429</v>
+        <v>117</v>
       </c>
       <c r="N7">
-        <v>592</v>
+        <v>131</v>
       </c>
       <c r="O7">
-        <v>172</v>
+        <v>38</v>
       </c>
       <c r="P7">
-        <v>313</v>
+        <v>97</v>
       </c>
       <c r="Q7">
-        <v>242</v>
+        <v>72</v>
       </c>
       <c r="R7">
-        <v>644</v>
+        <v>130</v>
       </c>
       <c r="S7">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7"/>
+      <c r="AL7"/>
+      <c r="AM7"/>
+      <c r="AN7"/>
+      <c r="AO7"/>
+      <c r="AP7"/>
+      <c r="AQ7"/>
+      <c r="AR7"/>
+      <c r="AS7"/>
+      <c r="AT7"/>
+      <c r="AU7"/>
+    </row>
+    <row r="8" x14ac:dyDescent="0.35">
       <c r="A8" s="17"/>
       <c r="B8" s="6"/>
       <c r="C8" s="11" t="str">
@@ -826,31 +882,59 @@
         <v>(0.086)</v>
       </c>
       <c r="L8">
-        <v>9.6475614097543613E-2</v>
+        <v>0.12303290414878398</v>
       </c>
       <c r="M8">
-        <v>0.15272338910644356</v>
+        <v>0.16738197424892703</v>
       </c>
       <c r="N8">
-        <v>0.21075115699537203</v>
+        <v>0.18741058655221746</v>
       </c>
       <c r="O8">
-        <v>6.1231755072979711E-2</v>
+        <v>0.054363376251788269</v>
       </c>
       <c r="P8">
-        <v>0.11142755428978283</v>
+        <v>0.13876967095851217</v>
       </c>
       <c r="Q8">
-        <v>8.6151655393378421E-2</v>
+        <v>0.10300429184549356</v>
       </c>
       <c r="R8">
-        <v>0.2292630829476682</v>
+        <v>0.1859799713876967</v>
       </c>
       <c r="S8">
-        <v>5.1975792096831612E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.04005722460658083</v>
+      </c>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+      <c r="AO8"/>
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
+      <c r="AS8"/>
+      <c r="AT8"/>
+      <c r="AU8"/>
+    </row>
+    <row r="9" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="7"/>
       <c r="C9" s="12">
@@ -870,7 +954,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" x14ac:dyDescent="0.35">
       <c r="A10" s="17"/>
       <c r="B10" s="6">
         <v>1</v>
@@ -892,37 +976,37 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="L10">
-        <v>7.1428571428571425E-2</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="M10">
-        <v>6.4220183486238536E-2</v>
+        <v>0.072916666666666671</v>
       </c>
       <c r="N10">
-        <v>2.7906976744186046E-2</v>
+        <v>0.042016806722689079</v>
       </c>
       <c r="O10">
-        <v>0.25</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="P10">
-        <v>0.79515769009626958</v>
+        <v>0.84950392562247212</v>
       </c>
       <c r="Q10">
-        <v>0.11161804742196123</v>
+        <v>0.40502502346319691</v>
       </c>
       <c r="R10">
-        <v>1.6862564906798411E-2</v>
+        <v>0.01258132777264883</v>
       </c>
       <c r="S10">
-        <v>0.11360117145877445</v>
+        <v>0.28815662793232538</v>
       </c>
       <c r="T10">
-        <v>1.7830538851595183E-2</v>
+        <v>0.020929163806872226</v>
       </c>
       <c r="U10">
-        <v>2.0688909375079462E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.0056087102572054967</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11" t="str">
@@ -942,19 +1026,25 @@
         <v>(0.076)</v>
       </c>
       <c r="L11">
-        <v>2.599497740543295E-2</v>
+        <v>0.026225335639063659</v>
       </c>
       <c r="M11">
-        <v>2.2006451765450526E-2</v>
+        <v>0.02515429572792378</v>
       </c>
       <c r="N11">
-        <v>1.1533897310887825E-2</v>
+        <v>0.019305731225769597</v>
       </c>
       <c r="O11">
-        <v>7.1794761521679878E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.093996557610129983</v>
+      </c>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+    </row>
+    <row r="12" x14ac:dyDescent="0.35">
       <c r="A12" s="17"/>
       <c r="B12" s="7"/>
       <c r="C12" s="12">
@@ -974,19 +1064,25 @@
         <v>146</v>
       </c>
       <c r="L12">
-        <v>584</v>
+        <v>183</v>
       </c>
       <c r="M12">
-        <v>671</v>
+        <v>189</v>
       </c>
       <c r="N12">
-        <v>1236</v>
+        <v>261</v>
       </c>
       <c r="O12">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+    </row>
+    <row r="13" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1007,19 +1103,25 @@
         <v>0.25</v>
       </c>
       <c r="L13">
-        <v>0.20790316838732645</v>
+        <v>0.26180257510729615</v>
       </c>
       <c r="M13">
-        <v>0.238875044499822</v>
+        <v>0.27038626609442062</v>
       </c>
       <c r="N13">
-        <v>0.44001423994304023</v>
+        <v>0.37339055793991416</v>
       </c>
       <c r="O13">
-        <v>0.11320754716981132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.094420600858369105</v>
+      </c>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+    </row>
+    <row r="14" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="11" t="str">
         <f>CONCATENATE("(",ROUND(L11,3),")")</f>
@@ -1038,7 +1140,7 @@
         <v>(0.072)</v>
       </c>
     </row>
-    <row r="15" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="13">
@@ -1058,8 +1160,8 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
+    <row r="19" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="19" t="s">
@@ -1069,7 +1171,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="10" t="s">
@@ -1085,7 +1187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="21" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
         <v>0</v>
       </c>
@@ -1111,16 +1213,16 @@
         <v>7</v>
       </c>
       <c r="M21">
-        <v>9.0496690936407762E-2</v>
+        <v>0.090496690936407762</v>
       </c>
       <c r="N21">
         <v>0.14444024088459634</v>
       </c>
       <c r="O21">
-        <v>-1.7064098515723318E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+        <v>-0.017064098515723318</v>
+      </c>
+    </row>
+    <row r="22" x14ac:dyDescent="0.35">
       <c r="A22" s="18"/>
       <c r="B22" s="7"/>
       <c r="C22" s="14" t="s">
@@ -1151,7 +1253,7 @@
         <v>0.14484859259458438</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" ht="15" customHeight="true" x14ac:dyDescent="0.35">
       <c r="A23" s="18"/>
       <c r="B23" s="6">
         <v>1</v>
@@ -1185,7 +1287,7 @@
         <v>0.16197325338401591</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" x14ac:dyDescent="0.35">
       <c r="A24" s="18"/>
       <c r="B24" s="7"/>
       <c r="C24" s="14" t="str">
@@ -1217,7 +1319,7 @@
         <v>0.13213925140111349</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>1</v>
       </c>
@@ -1240,16 +1342,16 @@
         <v>7</v>
       </c>
       <c r="M25">
-        <v>7.8085477077650969E-2</v>
+        <v>0.078085477077650969</v>
       </c>
       <c r="N25">
-        <v>6.892035878171851E-2</v>
+        <v>0.06892035878171851</v>
       </c>
       <c r="O25">
-        <v>-4.9080578885664986E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>-0.049080578885664986</v>
+      </c>
+    </row>
+    <row r="26" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="13" t="s">
@@ -1271,16 +1373,16 @@
         <v>7</v>
       </c>
       <c r="M26">
-        <v>7.5724436254924921E-2</v>
+        <v>0.075724436254924921</v>
       </c>
       <c r="N26">
-        <v>6.3410448251029705E-2</v>
+        <v>0.063410448251029705</v>
       </c>
       <c r="O26">
         <v>0.10038106690714045</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="27" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C5:F5"/>

</xml_diff>

<commit_message>
checkpoint before edits of tables and figues
</commit_message>
<xml_diff>
--- a/Tables/SS_learning.xlsx
+++ b/Tables/SS_learning.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CACF87-8992-4C25-8A93-124EBBEDC1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192F2534-7A8F-4147-99F6-B7011EACFC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25950" yWindow="-5850" windowWidth="21600" windowHeight="11235"/>
+    <workbookView xWindow="-25530" yWindow="-6105" windowWidth="23475" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_learning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="10">
   <si>
     <t>Default</t>
   </si>
@@ -56,6 +56,12 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>Comes next</t>
+  </si>
+  <si>
+    <t>Comes next and chooses</t>
+  </si>
 </sst>
 </file>
 
@@ -75,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -213,61 +219,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,102 +602,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:AU27"/>
+  <dimension ref="A5:AU55"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="5.1796875" style="1" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.7265625" style="11" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="10.6328125" style="11" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="10.7265625" style="11" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="11.54296875" style="11" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
       <c r="L5">
-        <v>0.068181818181818177</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="M5">
-        <v>0.072463768115942032</v>
+        <v>8.1967213114754092E-2</v>
       </c>
       <c r="N5">
-        <v>0.056603773584905662</v>
+        <v>5.6603773584905662E-2</v>
       </c>
       <c r="O5">
         <v>0.34782608695652173</v>
       </c>
       <c r="P5">
-        <v>0.066666666666666666</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="Q5">
-        <v>0.07407407407407407</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="R5">
-        <v>0.030303030303030304</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="S5">
         <v>0.23076923076923078</v>
       </c>
       <c r="T5">
-        <v>0.91138131955600066</v>
+        <v>0.85854409488166561</v>
       </c>
       <c r="U5">
-        <v>0.82461769586545186</v>
+        <v>0.57966709311602416</v>
       </c>
       <c r="V5">
-        <v>0.013564805283350202</v>
+        <v>3.0869969779705016E-2</v>
       </c>
       <c r="W5">
-        <v>0.97808876311225568</v>
+        <v>0.58372857096859843</v>
       </c>
       <c r="X5">
-        <v>0.92740043644858183</v>
+        <v>0.48577602808176823</v>
       </c>
       <c r="Y5">
-        <v>0.40634140811298913</v>
+        <v>0.29126462775567585</v>
       </c>
       <c r="Z5">
-        <v>0.21188197171210843</v>
+        <v>0.3021296384224309</v>
       </c>
       <c r="AA5">
-        <v>0.6949887776671434</v>
+        <v>0.55255115727476267</v>
       </c>
       <c r="AB5">
-        <v>0.01703624221488393</v>
+        <v>2.3669593255344037E-2</v>
       </c>
       <c r="AC5">
-        <v>0.89351820741680366</v>
+        <v>0.61380807584108843</v>
       </c>
       <c r="AD5">
-        <v>0.97916676003465897</v>
+        <v>0.48858370981741484</v>
       </c>
       <c r="AE5">
-        <v>0.25706829366071565</v>
+        <v>0.19959892061815485</v>
       </c>
       <c r="AF5">
-        <v>0.20872389344789977</v>
+        <v>0.2416401328199764</v>
       </c>
       <c r="AG5">
-        <v>0.011734441106661891</v>
+        <v>1.1734441106661891E-2</v>
       </c>
       <c r="AH5">
-        <v>0.80849018563525132</v>
+        <v>0.97923838101586369</v>
       </c>
       <c r="AI5">
-        <v>0.7723732627494021</v>
+        <v>0.80716341473210163</v>
       </c>
       <c r="AJ5">
         <v>0.50052526360916905</v>
@@ -688,37 +706,37 @@
         <v>0.16765757855540159</v>
       </c>
       <c r="AL5">
-        <v>0.0097748789346420884</v>
+        <v>5.7820282315942349E-3</v>
       </c>
       <c r="AM5">
-        <v>0.019449537871593373</v>
+        <v>8.6104895579723218E-3</v>
       </c>
       <c r="AN5">
-        <v>0.0021294895512379841</v>
+        <v>2.1294895512379841E-3</v>
       </c>
       <c r="AO5">
         <v>0.33038778340145369</v>
       </c>
       <c r="AP5">
-        <v>0.90850331591224687</v>
+        <v>0.833947811547461</v>
       </c>
       <c r="AQ5">
-        <v>0.3989092965964347</v>
+        <v>0.57020643420599493</v>
       </c>
       <c r="AR5">
-        <v>0.16780273381579652</v>
+        <v>0.13736953150950637</v>
       </c>
       <c r="AS5">
-        <v>0.43105846353394817</v>
+        <v>0.78178217520756665</v>
       </c>
       <c r="AT5">
-        <v>0.24135638719487112</v>
+        <v>0.15843604263411945</v>
       </c>
       <c r="AU5">
-        <v>0.087143941038846401</v>
-      </c>
-    </row>
-    <row r="6" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+        <v>8.7143941038846401E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="5"/>
       <c r="C6" s="10" t="s">
@@ -734,60 +752,32 @@
         <v>3</v>
       </c>
       <c r="L6">
-        <v>0.039704245002748807</v>
+        <v>5.2408251021902434E-2</v>
       </c>
       <c r="M6">
-        <v>0.030681682420916231</v>
+        <v>3.4266655915884417E-2</v>
       </c>
       <c r="N6">
-        <v>0.033153944802459187</v>
+        <v>3.3153944802459187E-2</v>
       </c>
       <c r="O6">
         <v>0.10218620161789856</v>
       </c>
       <c r="P6">
-        <v>0.036357553079168957</v>
+        <v>3.7974671151140206E-2</v>
       </c>
       <c r="Q6">
-        <v>0.051016228790772493</v>
+        <v>4.2259769034884334E-2</v>
       </c>
       <c r="R6">
-        <v>0.021609825968389312</v>
+        <v>2.1609825968389312E-2</v>
       </c>
       <c r="S6">
         <v>0.12483537131240699</v>
       </c>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-      <c r="AF6"/>
-      <c r="AG6"/>
-      <c r="AH6"/>
-      <c r="AI6"/>
-      <c r="AJ6"/>
-      <c r="AK6"/>
-      <c r="AL6"/>
-      <c r="AM6"/>
-      <c r="AN6"/>
-      <c r="AO6"/>
-      <c r="AP6"/>
-      <c r="AQ6"/>
-      <c r="AR6"/>
-      <c r="AS6"/>
-      <c r="AT6"/>
-      <c r="AU6"/>
-    </row>
-    <row r="7" ht="15" customHeight="true" thickTop="true" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+    </row>
+    <row r="7" spans="1:47" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="6">
@@ -795,25 +785,25 @@
       </c>
       <c r="C7" s="11">
         <f>ROUND(L5,3)</f>
-        <v>8.2000000000000003E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="D7" s="11">
         <f t="shared" ref="D7:F7" si="0">ROUND(M5,3)</f>
-        <v>6.3E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>4.2000000000000003E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="0"/>
-        <v>0.32400000000000001</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="L7">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="M7">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="N7">
         <v>131</v>
@@ -822,10 +812,10 @@
         <v>38</v>
       </c>
       <c r="P7">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="Q7">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="R7">
         <v>130</v>
@@ -833,241 +823,179 @@
       <c r="S7">
         <v>28</v>
       </c>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-      <c r="AC7"/>
-      <c r="AD7"/>
-      <c r="AE7"/>
-      <c r="AF7"/>
-      <c r="AG7"/>
-      <c r="AH7"/>
-      <c r="AI7"/>
-      <c r="AJ7"/>
-      <c r="AK7"/>
-      <c r="AL7"/>
-      <c r="AM7"/>
-      <c r="AN7"/>
-      <c r="AO7"/>
-      <c r="AP7"/>
-      <c r="AQ7"/>
-      <c r="AR7"/>
-      <c r="AS7"/>
-      <c r="AT7"/>
-      <c r="AU7"/>
-    </row>
-    <row r="8" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A8" s="18"/>
       <c r="B8" s="6"/>
       <c r="C8" s="11" t="str">
         <f>CONCATENATE("(",ROUND(L6,3),")")</f>
-        <v>(0.041)</v>
+        <v>(0.052)</v>
       </c>
       <c r="D8" s="11" t="str">
         <f t="shared" ref="D8:F8" si="1">CONCATENATE("(",ROUND(M6,3),")")</f>
-        <v>(0.026)</v>
+        <v>(0.034)</v>
       </c>
       <c r="E8" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(0.021)</v>
+        <v>(0.033)</v>
       </c>
       <c r="F8" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>(0.086)</v>
+        <v>(0.102)</v>
       </c>
       <c r="L8">
-        <v>0.12303290414878398</v>
+        <v>0.10126582278481013</v>
       </c>
       <c r="M8">
-        <v>0.16738197424892703</v>
+        <v>0.16297468354430381</v>
       </c>
       <c r="N8">
-        <v>0.18741058655221746</v>
+        <v>0.20727848101265822</v>
       </c>
       <c r="O8">
-        <v>0.054363376251788269</v>
+        <v>6.0126582278481014E-2</v>
       </c>
       <c r="P8">
-        <v>0.13876967095851217</v>
+        <v>0.12341772151898735</v>
       </c>
       <c r="Q8">
-        <v>0.10300429184549356</v>
+        <v>9.49367088607595E-2</v>
       </c>
       <c r="R8">
-        <v>0.1859799713876967</v>
+        <v>0.20569620253164558</v>
       </c>
       <c r="S8">
-        <v>0.04005722460658083</v>
-      </c>
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="Z8"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8"/>
-      <c r="AD8"/>
-      <c r="AE8"/>
-      <c r="AF8"/>
-      <c r="AG8"/>
-      <c r="AH8"/>
-      <c r="AI8"/>
-      <c r="AJ8"/>
-      <c r="AK8"/>
-      <c r="AL8"/>
-      <c r="AM8"/>
-      <c r="AN8"/>
-      <c r="AO8"/>
-      <c r="AP8"/>
-      <c r="AQ8"/>
-      <c r="AR8"/>
-      <c r="AS8"/>
-      <c r="AT8"/>
-      <c r="AU8"/>
-    </row>
-    <row r="9" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
+        <v>4.4303797468354431E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A9" s="18"/>
       <c r="B9" s="7"/>
       <c r="C9" s="12">
         <f>L7</f>
-        <v>271</v>
+        <v>64</v>
       </c>
       <c r="D9" s="12">
         <f t="shared" ref="D9:F9" si="2">M7</f>
-        <v>429</v>
+        <v>103</v>
       </c>
       <c r="E9" s="12">
         <f t="shared" si="2"/>
-        <v>592</v>
+        <v>131</v>
       </c>
       <c r="F9" s="12">
         <f t="shared" si="2"/>
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A10" s="18"/>
       <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="11">
         <f>ROUND(P5,3)</f>
-        <v>6.0999999999999999E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="D10" s="11">
         <f>ROUND(Q5,3)</f>
-        <v>6.9000000000000006E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="E10" s="11">
         <f>ROUND(R5,3)</f>
-        <v>1.7000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F10" s="11">
         <f>ROUND(S5,3)</f>
-        <v>0.13600000000000001</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="L10">
-        <v>0.06741573033707865</v>
+        <v>7.2463768115942032E-2</v>
       </c>
       <c r="M10">
-        <v>0.072916666666666671</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="N10">
-        <v>0.042016806722689079</v>
+        <v>4.2016806722689079E-2</v>
       </c>
       <c r="O10">
         <v>0.30555555555555558</v>
       </c>
       <c r="P10">
-        <v>0.84950392562247212</v>
+        <v>0.97711458380152483</v>
       </c>
       <c r="Q10">
-        <v>0.40502502346319691</v>
+        <v>0.3826614156190562</v>
       </c>
       <c r="R10">
-        <v>0.01258132777264883</v>
+        <v>1.4687606629663225E-2</v>
       </c>
       <c r="S10">
-        <v>0.28815662793232538</v>
+        <v>0.33107059638501168</v>
       </c>
       <c r="T10">
-        <v>0.020929163806872226</v>
+        <v>2.1684011362586381E-2</v>
       </c>
       <c r="U10">
-        <v>0.0056087102572054967</v>
-      </c>
-    </row>
-    <row r="11" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
+        <v>5.6087102572054967E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A11" s="18"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11" t="str">
         <f>CONCATENATE("(",ROUND(P6,3),")")</f>
-        <v>(0.034)</v>
+        <v>(0.038)</v>
       </c>
       <c r="D11" s="11" t="str">
         <f>CONCATENATE("(",ROUND(Q6,3),")")</f>
-        <v>(0.047)</v>
+        <v>(0.042)</v>
       </c>
       <c r="E11" s="11" t="str">
         <f>CONCATENATE("(",ROUND(R6,3),")")</f>
-        <v>(0.012)</v>
+        <v>(0.022)</v>
       </c>
       <c r="F11" s="11" t="str">
         <f>CONCATENATE("(",ROUND(S6,3),")")</f>
-        <v>(0.076)</v>
+        <v>(0.125)</v>
       </c>
       <c r="L11">
-        <v>0.026225335639063659</v>
+        <v>3.1826575371887406E-2</v>
       </c>
       <c r="M11">
-        <v>0.02515429572792378</v>
+        <v>2.6893171679313016E-2</v>
       </c>
       <c r="N11">
-        <v>0.019305731225769597</v>
+        <v>1.9305731225769597E-2</v>
       </c>
       <c r="O11">
-        <v>0.093996557610129983</v>
-      </c>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
-      <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-    </row>
-    <row r="12" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
+        <v>9.3996557610129983E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A12" s="18"/>
       <c r="B12" s="7"/>
       <c r="C12" s="12">
         <f>P7</f>
-        <v>313</v>
+        <v>78</v>
       </c>
       <c r="D12" s="12">
         <f>Q7</f>
-        <v>242</v>
+        <v>60</v>
       </c>
       <c r="E12" s="12">
         <f>R7</f>
-        <v>644</v>
+        <v>130</v>
       </c>
       <c r="F12" s="12">
         <f>S7</f>
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="L12">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="M12">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="N12">
         <v>261</v>
@@ -1075,103 +1003,91 @@
       <c r="O12">
         <v>66</v>
       </c>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
-      <c r="T12"/>
-      <c r="U12"/>
-    </row>
-    <row r="13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="11">
         <f>ROUND(L10,3)</f>
-        <v>7.0999999999999994E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D13" s="11">
         <f>ROUND(M10,3)</f>
-        <v>6.4000000000000001E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E13" s="11">
         <f>ROUND(N10,3)</f>
-        <v>2.8000000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F13" s="11">
         <f>ROUND(O10,3)</f>
-        <v>0.25</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="L13">
-        <v>0.26180257510729615</v>
+        <v>0.22468354430379747</v>
       </c>
       <c r="M13">
-        <v>0.27038626609442062</v>
+        <v>0.25791139240506328</v>
       </c>
       <c r="N13">
-        <v>0.37339055793991416</v>
+        <v>0.41297468354430378</v>
       </c>
       <c r="O13">
-        <v>0.094420600858369105</v>
-      </c>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="S13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-    </row>
-    <row r="14" x14ac:dyDescent="0.35">
+        <v>0.10443037974683544</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="11" t="str">
         <f>CONCATENATE("(",ROUND(L11,3),")")</f>
-        <v>(0.026)</v>
+        <v>(0.032)</v>
       </c>
       <c r="D14" s="11" t="str">
         <f>CONCATENATE("(",ROUND(M11,3),")")</f>
-        <v>(0.022)</v>
+        <v>(0.027)</v>
       </c>
       <c r="E14" s="11" t="str">
         <f>CONCATENATE("(",ROUND(N11,3),")")</f>
-        <v>(0.012)</v>
+        <v>(0.019)</v>
       </c>
       <c r="F14" s="11" t="str">
         <f>CONCATENATE("(",ROUND(O11,3),")")</f>
-        <v>(0.072)</v>
-      </c>
-    </row>
-    <row r="15" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+        <v>(0.094)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="13">
         <f>L12</f>
-        <v>584</v>
+        <v>142</v>
       </c>
       <c r="D15" s="13">
         <f>M12</f>
-        <v>671</v>
+        <v>163</v>
       </c>
       <c r="E15" s="13">
         <f>N12</f>
-        <v>1236</v>
+        <v>261</v>
       </c>
       <c r="F15" s="13">
         <f>O12</f>
-        <v>318</v>
-      </c>
-    </row>
-    <row r="16" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
-    <row r="19" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-    </row>
-    <row r="20" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="10" t="s">
@@ -1187,8 +1103,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" ht="15" thickTop="true" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="6">
@@ -1213,17 +1129,17 @@
         <v>7</v>
       </c>
       <c r="M21">
-        <v>0.090496690936407762</v>
+        <v>9.0496690936407762E-2</v>
       </c>
       <c r="N21">
         <v>0.14444024088459634</v>
       </c>
       <c r="O21">
-        <v>-0.017064098515723318</v>
-      </c>
-    </row>
-    <row r="22" x14ac:dyDescent="0.35">
-      <c r="A22" s="18"/>
+        <v>-1.7064098515723318E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A22" s="19"/>
       <c r="B22" s="7"/>
       <c r="C22" s="14" t="s">
         <v>7</v>
@@ -1253,8 +1169,8 @@
         <v>0.14484859259458438</v>
       </c>
     </row>
-    <row r="23" ht="15" customHeight="true" x14ac:dyDescent="0.35">
-      <c r="A23" s="18"/>
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19"/>
       <c r="B23" s="6">
         <v>1</v>
       </c>
@@ -1287,8 +1203,8 @@
         <v>0.16197325338401591</v>
       </c>
     </row>
-    <row r="24" x14ac:dyDescent="0.35">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A24" s="19"/>
       <c r="B24" s="7"/>
       <c r="C24" s="14" t="str">
         <f>CONCATENATE("(",ROUND(L24,3),")")</f>
@@ -1319,7 +1235,7 @@
         <v>0.13213925140111349</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>1</v>
       </c>
@@ -1342,16 +1258,16 @@
         <v>7</v>
       </c>
       <c r="M25">
-        <v>0.078085477077650969</v>
+        <v>7.8085477077650969E-2</v>
       </c>
       <c r="N25">
-        <v>0.06892035878171851</v>
+        <v>6.892035878171851E-2</v>
       </c>
       <c r="O25">
-        <v>-0.049080578885664986</v>
-      </c>
-    </row>
-    <row r="26" ht="15" thickBot="true" x14ac:dyDescent="0.4">
+        <v>-4.9080578885664986E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="13" t="s">
@@ -1373,22 +1289,773 @@
         <v>7</v>
       </c>
       <c r="M26">
-        <v>0.075724436254924921</v>
+        <v>7.5724436254924921E-2</v>
       </c>
       <c r="N26">
-        <v>0.063410448251029705</v>
+        <v>6.3410448251029705E-2</v>
       </c>
       <c r="O26">
         <v>0.10038106690714045</v>
       </c>
     </row>
-    <row r="27" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="11">
+        <f>ROUND(L31,3)</f>
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="D31" s="11">
+        <f t="shared" ref="D31:F31" si="3">ROUND(M31,3)</f>
+        <v>0.215</v>
+      </c>
+      <c r="E31" s="11">
+        <f t="shared" si="3"/>
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F31" s="11">
+        <f t="shared" si="3"/>
+        <v>0.215</v>
+      </c>
+      <c r="L31">
+        <v>0.21259198691741618</v>
+      </c>
+      <c r="M31">
+        <v>0.21549295774647886</v>
+      </c>
+      <c r="N31">
+        <v>0.22906403940886699</v>
+      </c>
+      <c r="O31">
+        <v>0.2153846153846154</v>
+      </c>
+      <c r="P31">
+        <v>0.92117487590348524</v>
+      </c>
+      <c r="Q31">
+        <v>0.55591760534177981</v>
+      </c>
+      <c r="R31">
+        <v>0.92817544553152997</v>
+      </c>
+      <c r="S31">
+        <v>0.57907584140368695</v>
+      </c>
+      <c r="T31">
+        <v>0.99689640239812527</v>
+      </c>
+      <c r="U31">
+        <v>0.542154442615294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C32" s="11" t="str">
+        <f>CONCATENATE("(",ROUND(L32,3),")")</f>
+        <v>(0.023)</v>
+      </c>
+      <c r="D32" s="11" t="str">
+        <f t="shared" ref="D32:F32" si="4">CONCATENATE("(",ROUND(M32,3),")")</f>
+        <v>(0.018)</v>
+      </c>
+      <c r="E32" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>(0.016)</v>
+      </c>
+      <c r="F32" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>(0.021)</v>
+      </c>
+      <c r="L32">
+        <v>2.2872080473634156E-2</v>
+      </c>
+      <c r="M32">
+        <v>1.8399530077354433E-2</v>
+      </c>
+      <c r="N32">
+        <v>1.6174356828906031E-2</v>
+      </c>
+      <c r="O32">
+        <v>2.0950673136672596E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="C33" s="15">
+        <f>L33</f>
+        <v>1223</v>
+      </c>
+      <c r="D33" s="15">
+        <f t="shared" ref="D33:F33" si="5">M33</f>
+        <v>1420</v>
+      </c>
+      <c r="E33" s="15">
+        <f t="shared" si="5"/>
+        <v>2436</v>
+      </c>
+      <c r="F33" s="15">
+        <f t="shared" si="5"/>
+        <v>650</v>
+      </c>
+      <c r="L33">
+        <v>1223</v>
+      </c>
+      <c r="M33">
+        <v>1420</v>
+      </c>
+      <c r="N33">
+        <v>2436</v>
+      </c>
+      <c r="O33">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <v>0.21347530109966836</v>
+      </c>
+      <c r="M34">
+        <v>0.24786175597835575</v>
+      </c>
+      <c r="N34">
+        <v>0.42520509687554547</v>
+      </c>
+      <c r="O34">
+        <v>0.11345784604643044</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C35" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="11">
+        <f>ROUND(L37,3)</f>
+        <v>0.115</v>
+      </c>
+      <c r="D37" s="11">
+        <f t="shared" ref="D37:F37" si="6">ROUND(M37,3)</f>
+        <v>0.115</v>
+      </c>
+      <c r="E37" s="11">
+        <f t="shared" si="6"/>
+        <v>0.107</v>
+      </c>
+      <c r="F37" s="11">
+        <f t="shared" si="6"/>
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="L37">
+        <v>0.11529026982829109</v>
+      </c>
+      <c r="M37">
+        <v>0.11549295774647887</v>
+      </c>
+      <c r="N37">
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="O37">
+        <v>0.10153846153846154</v>
+      </c>
+      <c r="P37">
+        <v>0.99146136885369551</v>
+      </c>
+      <c r="Q37">
+        <v>0.64985571800679431</v>
+      </c>
+      <c r="R37">
+        <v>0.48365525720350733</v>
+      </c>
+      <c r="S37">
+        <v>0.58011910619982388</v>
+      </c>
+      <c r="T37">
+        <v>0.41336221771886927</v>
+      </c>
+      <c r="U37">
+        <v>0.69233383748107036</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="C38" s="11" t="str">
+        <f>CONCATENATE("(",ROUND(L38,3),")")</f>
+        <v>(0.015)</v>
+      </c>
+      <c r="D38" s="11" t="str">
+        <f t="shared" ref="D38:F38" si="7">CONCATENATE("(",ROUND(M38,3),")")</f>
+        <v>(0.012)</v>
+      </c>
+      <c r="E38" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>(0.01)</v>
+      </c>
+      <c r="F38" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>(0.013)</v>
+      </c>
+      <c r="L38">
+        <v>1.5073492993024722E-2</v>
+      </c>
+      <c r="M38">
+        <v>1.150794809496546E-2</v>
+      </c>
+      <c r="N38">
+        <v>9.8004940779611721E-3</v>
+      </c>
+      <c r="O38">
+        <v>1.2599605142795837E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="C39" s="15">
+        <f>L39</f>
+        <v>1223</v>
+      </c>
+      <c r="D39" s="15">
+        <f t="shared" ref="D39:F39" si="8">M39</f>
+        <v>1420</v>
+      </c>
+      <c r="E39" s="15">
+        <f t="shared" si="8"/>
+        <v>2436</v>
+      </c>
+      <c r="F39" s="15">
+        <f t="shared" si="8"/>
+        <v>650</v>
+      </c>
+      <c r="L39">
+        <v>1223</v>
+      </c>
+      <c r="M39">
+        <v>1420</v>
+      </c>
+      <c r="N39">
+        <v>2436</v>
+      </c>
+      <c r="O39">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="L40">
+        <v>0.21347530109966836</v>
+      </c>
+      <c r="M40">
+        <v>0.24786175597835575</v>
+      </c>
+      <c r="N40">
+        <v>0.42520509687554547</v>
+      </c>
+      <c r="O40">
+        <v>0.11345784604643044</v>
+      </c>
+    </row>
+    <row r="44" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="2"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+    </row>
+    <row r="45" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="3"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="6">
+        <v>0</v>
+      </c>
+      <c r="C46" s="11">
+        <f>ROUND(L46,3)</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D46" s="11">
+        <f t="shared" ref="D46:F46" si="9">ROUND(M46,3)</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E46" s="11">
+        <f t="shared" si="9"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F46" s="11">
+        <f t="shared" si="9"/>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="L46">
+        <v>6.0362173038229373E-3</v>
+      </c>
+      <c r="M46">
+        <v>8.7939698492462311E-3</v>
+      </c>
+      <c r="N46">
+        <v>3.8204393505253103E-3</v>
+      </c>
+      <c r="O46">
+        <v>3.3112582781456956E-2</v>
+      </c>
+      <c r="P46">
+        <v>4.1322314049586778E-3</v>
+      </c>
+      <c r="Q46">
+        <v>1.6025641025641025E-3</v>
+      </c>
+      <c r="R46">
+        <v>1.4398848092152627E-3</v>
+      </c>
+      <c r="S46">
+        <v>1.4367816091954023E-2</v>
+      </c>
+      <c r="T46">
+        <v>0.58969992750037326</v>
+      </c>
+      <c r="U46">
+        <v>0.55250971508421043</v>
+      </c>
+      <c r="V46">
+        <v>1.8407068204269555E-2</v>
+      </c>
+      <c r="W46">
+        <v>0.62862683302623001</v>
+      </c>
+      <c r="X46">
+        <v>0.21406078147350102</v>
+      </c>
+      <c r="Y46">
+        <v>0.17229966554926596</v>
+      </c>
+      <c r="Z46">
+        <v>0.24649790188440676</v>
+      </c>
+      <c r="AA46">
+        <v>0.26007222690715609</v>
+      </c>
+      <c r="AB46">
+        <v>3.7829755416234012E-2</v>
+      </c>
+      <c r="AC46">
+        <v>0.35548481337955851</v>
+      </c>
+      <c r="AD46">
+        <v>0.10559072620397023</v>
+      </c>
+      <c r="AE46">
+        <v>7.408212708045564E-2</v>
+      </c>
+      <c r="AF46">
+        <v>0.46089115939483838</v>
+      </c>
+      <c r="AG46">
+        <v>9.0264384448070067E-3</v>
+      </c>
+      <c r="AH46">
+        <v>0.93152462716313278</v>
+      </c>
+      <c r="AI46">
+        <v>0.36720008178973473</v>
+      </c>
+      <c r="AJ46">
+        <v>0.27444268091051138</v>
+      </c>
+      <c r="AK46">
+        <v>0.11877671030537655</v>
+      </c>
+      <c r="AL46">
+        <v>1.1481977701865318E-2</v>
+      </c>
+      <c r="AM46">
+        <v>4.8019108587179253E-3</v>
+      </c>
+      <c r="AN46">
+        <v>4.4813094464451761E-3</v>
+      </c>
+      <c r="AO46">
+        <v>9.829865334150048E-2</v>
+      </c>
+      <c r="AP46">
+        <v>0.46430199723748322</v>
+      </c>
+      <c r="AQ46">
+        <v>0.40773426203941454</v>
+      </c>
+      <c r="AR46">
+        <v>0.15189501258061022</v>
+      </c>
+      <c r="AS46">
+        <v>0.9300658344299777</v>
+      </c>
+      <c r="AT46">
+        <v>5.4480493222876347E-2</v>
+      </c>
+      <c r="AU46">
+        <v>4.8449546729351228E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A47" s="18"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="11" t="str">
+        <f>CONCATENATE("(",ROUND(L47,3),")")</f>
+        <v>(0.003)</v>
+      </c>
+      <c r="D47" s="11" t="str">
+        <f t="shared" ref="D47:F47" si="10">CONCATENATE("(",ROUND(M47,3),")")</f>
+        <v>(0.004)</v>
+      </c>
+      <c r="E47" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>(0.002)</v>
+      </c>
+      <c r="F47" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>(0.011)</v>
+      </c>
+      <c r="L47">
+        <v>3.2097112650795938E-3</v>
+      </c>
+      <c r="M47">
+        <v>3.9863207725839176E-3</v>
+      </c>
+      <c r="N47">
+        <v>1.912172940715021E-3</v>
+      </c>
+      <c r="O47">
+        <v>1.0940016107615524E-2</v>
+      </c>
+      <c r="P47">
+        <v>3.0920931358299391E-3</v>
+      </c>
+      <c r="Q47">
+        <v>1.547585312409367E-3</v>
+      </c>
+      <c r="R47">
+        <v>1.0274815285485808E-3</v>
+      </c>
+      <c r="S47">
+        <v>6.4219294058349254E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A48" s="18"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="12">
+        <f>L48</f>
+        <v>800</v>
+      </c>
+      <c r="D48" s="12">
+        <f t="shared" ref="D48:F48" si="11">M48</f>
+        <v>1504</v>
+      </c>
+      <c r="E48" s="12">
+        <f t="shared" si="11"/>
+        <v>1763</v>
+      </c>
+      <c r="F48" s="12">
+        <f t="shared" si="11"/>
+        <v>534</v>
+      </c>
+      <c r="L48">
+        <v>800</v>
+      </c>
+      <c r="M48">
+        <v>1504</v>
+      </c>
+      <c r="N48">
+        <v>1763</v>
+      </c>
+      <c r="O48">
+        <v>534</v>
+      </c>
+      <c r="P48">
+        <v>1122</v>
+      </c>
+      <c r="Q48">
+        <v>946</v>
+      </c>
+      <c r="R48">
+        <v>2082</v>
+      </c>
+      <c r="S48">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A49" s="18"/>
+      <c r="B49" s="6">
+        <v>1</v>
+      </c>
+      <c r="C49" s="11">
+        <f>ROUND(P46,3)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D49" s="11">
+        <f t="shared" ref="D49:F49" si="12">ROUND(Q46,3)</f>
+        <v>2E-3</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" si="12"/>
+        <v>1E-3</v>
+      </c>
+      <c r="F49" s="11">
+        <f t="shared" si="12"/>
+        <v>1.4E-2</v>
+      </c>
+      <c r="L49">
+        <v>8.6673889490790898E-2</v>
+      </c>
+      <c r="M49">
+        <v>0.1629469122426869</v>
+      </c>
+      <c r="N49">
+        <v>0.19100758396533044</v>
+      </c>
+      <c r="O49">
+        <v>5.7854821235102924E-2</v>
+      </c>
+      <c r="P49">
+        <v>0.12156013001083424</v>
+      </c>
+      <c r="Q49">
+        <v>0.10249187432286024</v>
+      </c>
+      <c r="R49">
+        <v>0.22556879739978331</v>
+      </c>
+      <c r="S49">
+        <v>5.1895991332611052E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A50" s="18"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="11" t="str">
+        <f>CONCATENATE("(",ROUND(P47,3),")")</f>
+        <v>(0.003)</v>
+      </c>
+      <c r="D50" s="11" t="str">
+        <f t="shared" ref="D50:F50" si="13">CONCATENATE("(",ROUND(Q47,3),")")</f>
+        <v>(0.002)</v>
+      </c>
+      <c r="E50" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>(0.001)</v>
+      </c>
+      <c r="F50" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>(0.006)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A51" s="18"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="12">
+        <f>P48</f>
+        <v>1122</v>
+      </c>
+      <c r="D51" s="12">
+        <f t="shared" ref="D51:F51" si="14">Q48</f>
+        <v>946</v>
+      </c>
+      <c r="E51" s="12">
+        <f t="shared" si="14"/>
+        <v>2082</v>
+      </c>
+      <c r="F51" s="12">
+        <f t="shared" si="14"/>
+        <v>479</v>
+      </c>
+      <c r="L51">
+        <v>4.9059689288634507E-3</v>
+      </c>
+      <c r="M51">
+        <v>5.6338028169014088E-3</v>
+      </c>
+      <c r="N51">
+        <v>2.4630541871921183E-3</v>
+      </c>
+      <c r="O51">
+        <v>2.3076923076923078E-2</v>
+      </c>
+      <c r="P51">
+        <v>0.82852764560199688</v>
+      </c>
+      <c r="Q51">
+        <v>0.36171005565460346</v>
+      </c>
+      <c r="R51">
+        <v>1.3382051452367592E-2</v>
+      </c>
+      <c r="S51">
+        <v>0.20130660961618221</v>
+      </c>
+      <c r="T51">
+        <v>1.6472860420285621E-2</v>
+      </c>
+      <c r="U51">
+        <v>3.4068444991565811E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B52" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="11">
+        <f>ROUND(L51,3)</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D52" s="11">
+        <f t="shared" ref="D52:F52" si="15">ROUND(M51,3)</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E52" s="11">
+        <f t="shared" si="15"/>
+        <v>2E-3</v>
+      </c>
+      <c r="F52" s="11">
+        <f t="shared" si="15"/>
+        <v>2.3E-2</v>
+      </c>
+      <c r="L52">
+        <v>2.4848151172649161E-3</v>
+      </c>
+      <c r="M52">
+        <v>2.2685807958589595E-3</v>
+      </c>
+      <c r="N52">
+        <v>1.011381433704327E-3</v>
+      </c>
+      <c r="O52">
+        <v>6.8577616757890571E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B53" s="6"/>
+      <c r="C53" s="11" t="str">
+        <f>CONCATENATE("(",ROUND(L52,3),")")</f>
+        <v>(0.002)</v>
+      </c>
+      <c r="D53" s="11" t="str">
+        <f t="shared" ref="D53:F53" si="16">CONCATENATE("(",ROUND(M52,3),")")</f>
+        <v>(0.002)</v>
+      </c>
+      <c r="E53" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>(0.001)</v>
+      </c>
+      <c r="F53" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>(0.007)</v>
+      </c>
+      <c r="L53">
+        <v>1922</v>
+      </c>
+      <c r="M53">
+        <v>2450</v>
+      </c>
+      <c r="N53">
+        <v>3845</v>
+      </c>
+      <c r="O53">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="8"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="13">
+        <f>L53</f>
+        <v>1922</v>
+      </c>
+      <c r="D54" s="13">
+        <f t="shared" ref="D54:F54" si="17">M53</f>
+        <v>2450</v>
+      </c>
+      <c r="E54" s="13">
+        <f t="shared" si="17"/>
+        <v>3845</v>
+      </c>
+      <c r="F54" s="13">
+        <f t="shared" si="17"/>
+        <v>1013</v>
+      </c>
+      <c r="L54">
+        <v>0.20823401950162512</v>
+      </c>
+      <c r="M54">
+        <v>0.26543878656554715</v>
+      </c>
+      <c r="N54">
+        <v>0.41657638136511377</v>
+      </c>
+      <c r="O54">
+        <v>0.10975081256771398</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="C35:F35"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learning by not doing analysis & replace eff_cost_loan with APR
</commit_message>
<xml_diff>
--- a/Tables/SS_learning.xlsx
+++ b/Tables/SS_learning.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192F2534-7A8F-4147-99F6-B7011EACFC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25530" yWindow="-6105" windowWidth="23475" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25530" yWindow="-6105" windowWidth="23475" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="SS_learning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -234,58 +234,58 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -604,21 +604,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:AU55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="5.1796875" style="1" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.7265625" style="11" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="10.6328125" style="11" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="10.7265625" style="11" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="11.54296875" style="11" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="16" t="s">
@@ -628,43 +628,43 @@
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="L5">
-        <v>9.0909090909090912E-2</v>
+        <v>0.090909090909090912</v>
       </c>
       <c r="M5">
-        <v>8.1967213114754092E-2</v>
+        <v>0.083333333333333329</v>
       </c>
       <c r="N5">
-        <v>5.6603773584905662E-2</v>
+        <v>0.056603773584905662</v>
       </c>
       <c r="O5">
         <v>0.34782608695652173</v>
       </c>
       <c r="P5">
-        <v>5.5555555555555552E-2</v>
+        <v>0.055555555555555552</v>
       </c>
       <c r="Q5">
-        <v>4.3478260869565216E-2</v>
+        <v>0.041666666666666664</v>
       </c>
       <c r="R5">
-        <v>3.0303030303030304E-2</v>
+        <v>0.030303030303030304</v>
       </c>
       <c r="S5">
         <v>0.23076923076923078</v>
       </c>
       <c r="T5">
-        <v>0.85854409488166561</v>
+        <v>0.87902374585065202</v>
       </c>
       <c r="U5">
         <v>0.57966709311602416</v>
       </c>
       <c r="V5">
-        <v>3.0869969779705016E-2</v>
+        <v>0.030869969779705016</v>
       </c>
       <c r="W5">
         <v>0.58372857096859843</v>
       </c>
       <c r="X5">
-        <v>0.48577602808176823</v>
+        <v>0.46441312409481539</v>
       </c>
       <c r="Y5">
         <v>0.29126462775567585</v>
@@ -673,31 +673,31 @@
         <v>0.3021296384224309</v>
       </c>
       <c r="AA5">
-        <v>0.55255115727476267</v>
+        <v>0.53092999993579626</v>
       </c>
       <c r="AB5">
-        <v>2.3669593255344037E-2</v>
+        <v>0.02422401611960389</v>
       </c>
       <c r="AC5">
-        <v>0.61380807584108843</v>
+        <v>0.59547528838212915</v>
       </c>
       <c r="AD5">
-        <v>0.48858370981741484</v>
+        <v>0.44093450044819915</v>
       </c>
       <c r="AE5">
-        <v>0.19959892061815485</v>
+        <v>0.18785711147425319</v>
       </c>
       <c r="AF5">
-        <v>0.2416401328199764</v>
+        <v>0.24656250004920716</v>
       </c>
       <c r="AG5">
-        <v>1.1734441106661891E-2</v>
+        <v>0.011734441106661891</v>
       </c>
       <c r="AH5">
         <v>0.97923838101586369</v>
       </c>
       <c r="AI5">
-        <v>0.80716341473210163</v>
+        <v>0.77673274338213938</v>
       </c>
       <c r="AJ5">
         <v>0.50052526360916905</v>
@@ -706,19 +706,19 @@
         <v>0.16765757855540159</v>
       </c>
       <c r="AL5">
-        <v>5.7820282315942349E-3</v>
+        <v>0.0057820282315942349</v>
       </c>
       <c r="AM5">
-        <v>8.6104895579723218E-3</v>
+        <v>0.0080300769665272199</v>
       </c>
       <c r="AN5">
-        <v>2.1294895512379841E-3</v>
+        <v>0.0021294895512379841</v>
       </c>
       <c r="AO5">
         <v>0.33038778340145369</v>
       </c>
       <c r="AP5">
-        <v>0.833947811547461</v>
+        <v>0.80577770089818301</v>
       </c>
       <c r="AQ5">
         <v>0.57020643420599493</v>
@@ -727,16 +727,16 @@
         <v>0.13736953150950637</v>
       </c>
       <c r="AS5">
-        <v>0.78178217520756665</v>
+        <v>0.80607444033965014</v>
       </c>
       <c r="AT5">
-        <v>0.15843604263411945</v>
+        <v>0.15348653167595988</v>
       </c>
       <c r="AU5">
-        <v>8.7143941038846401E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.087143941038846401</v>
+      </c>
+    </row>
+    <row r="6" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="5"/>
       <c r="C6" s="10" t="s">
@@ -752,31 +752,59 @@
         <v>3</v>
       </c>
       <c r="L6">
-        <v>5.2408251021902434E-2</v>
+        <v>0.052408251021902434</v>
       </c>
       <c r="M6">
-        <v>3.4266655915884417E-2</v>
+        <v>0.034246744460938755</v>
       </c>
       <c r="N6">
-        <v>3.3153944802459187E-2</v>
+        <v>0.033153944802459187</v>
       </c>
       <c r="O6">
         <v>0.10218620161789856</v>
       </c>
       <c r="P6">
-        <v>3.7974671151140206E-2</v>
+        <v>0.037974671151140206</v>
       </c>
       <c r="Q6">
-        <v>4.2259769034884334E-2</v>
+        <v>0.040815447263188462</v>
       </c>
       <c r="R6">
-        <v>2.1609825968389312E-2</v>
+        <v>0.021609825968389312</v>
       </c>
       <c r="S6">
         <v>0.12483537131240699</v>
       </c>
-    </row>
-    <row r="7" spans="1:47" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6"/>
+      <c r="AL6"/>
+      <c r="AM6"/>
+      <c r="AN6"/>
+      <c r="AO6"/>
+      <c r="AP6"/>
+      <c r="AQ6"/>
+      <c r="AR6"/>
+      <c r="AS6"/>
+      <c r="AT6"/>
+      <c r="AU6"/>
+    </row>
+    <row r="7" ht="15" customHeight="true" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
@@ -800,31 +828,59 @@
         <v>0.34799999999999998</v>
       </c>
       <c r="L7">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M7">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N7">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="O7">
         <v>38</v>
       </c>
       <c r="P7">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q7">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R7">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="S7">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7"/>
+      <c r="AL7"/>
+      <c r="AM7"/>
+      <c r="AN7"/>
+      <c r="AO7"/>
+      <c r="AP7"/>
+      <c r="AQ7"/>
+      <c r="AR7"/>
+      <c r="AS7"/>
+      <c r="AT7"/>
+      <c r="AU7"/>
+    </row>
+    <row r="8" x14ac:dyDescent="0.35">
       <c r="A8" s="18"/>
       <c r="B8" s="6"/>
       <c r="C8" s="11" t="str">
@@ -844,31 +900,59 @@
         <v>(0.102)</v>
       </c>
       <c r="L8">
-        <v>0.10126582278481013</v>
+        <v>0.097946287519747238</v>
       </c>
       <c r="M8">
-        <v>0.16297468354430381</v>
+        <v>0.16113744075829384</v>
       </c>
       <c r="N8">
-        <v>0.20727848101265822</v>
+        <v>0.20853080568720378</v>
       </c>
       <c r="O8">
-        <v>6.0126582278481014E-2</v>
+        <v>0.060031595576619273</v>
       </c>
       <c r="P8">
-        <v>0.12341772151898735</v>
+        <v>0.12480252764612954</v>
       </c>
       <c r="Q8">
-        <v>9.49367088607595E-2</v>
+        <v>0.096366508688783575</v>
       </c>
       <c r="R8">
-        <v>0.20569620253164558</v>
+        <v>0.20695102685624012</v>
       </c>
       <c r="S8">
-        <v>4.4303797468354431E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.044233807266982623</v>
+      </c>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+      <c r="AO8"/>
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
+      <c r="AS8"/>
+      <c r="AT8"/>
+      <c r="AU8"/>
+    </row>
+    <row r="9" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
       <c r="B9" s="7"/>
       <c r="C9" s="12">
@@ -888,7 +972,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" x14ac:dyDescent="0.35">
       <c r="A10" s="18"/>
       <c r="B10" s="6">
         <v>1</v>
@@ -910,37 +994,37 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="L10">
-        <v>7.2463768115942032E-2</v>
+        <v>0.072463768115942032</v>
       </c>
       <c r="M10">
-        <v>7.1428571428571425E-2</v>
+        <v>0.071428571428571425</v>
       </c>
       <c r="N10">
-        <v>4.2016806722689079E-2</v>
+        <v>0.042016806722689079</v>
       </c>
       <c r="O10">
         <v>0.30555555555555558</v>
       </c>
       <c r="P10">
-        <v>0.97711458380152483</v>
+        <v>0.97712458681109271</v>
       </c>
       <c r="Q10">
         <v>0.3826614156190562</v>
       </c>
       <c r="R10">
-        <v>1.4687606629663225E-2</v>
+        <v>0.014687606629663343</v>
       </c>
       <c r="S10">
-        <v>0.33107059638501168</v>
+        <v>0.33201610969502537</v>
       </c>
       <c r="T10">
-        <v>2.1684011362586381E-2</v>
+        <v>0.021797449618275004</v>
       </c>
       <c r="U10">
-        <v>5.6087102572054967E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.0056087102572054967</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11" t="str">
@@ -960,19 +1044,25 @@
         <v>(0.125)</v>
       </c>
       <c r="L11">
-        <v>3.1826575371887406E-2</v>
+        <v>0.031826575371887406</v>
       </c>
       <c r="M11">
-        <v>2.6893171679313016E-2</v>
+        <v>0.026948111821723696</v>
       </c>
       <c r="N11">
-        <v>1.9305731225769597E-2</v>
+        <v>0.019305731225769597</v>
       </c>
       <c r="O11">
-        <v>9.3996557610129983E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.093996557610129983</v>
+      </c>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+    </row>
+    <row r="12" x14ac:dyDescent="0.35">
       <c r="A12" s="18"/>
       <c r="B12" s="7"/>
       <c r="C12" s="12">
@@ -992,19 +1082,25 @@
         <v>28</v>
       </c>
       <c r="L12">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M12">
         <v>163</v>
       </c>
       <c r="N12">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="O12">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+    </row>
+    <row r="13" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1025,19 +1121,25 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="L13">
-        <v>0.22468354430379747</v>
+        <v>0.22274881516587677</v>
       </c>
       <c r="M13">
-        <v>0.25791139240506328</v>
+        <v>0.25750394944707738</v>
       </c>
       <c r="N13">
-        <v>0.41297468354430378</v>
+        <v>0.4154818325434439</v>
       </c>
       <c r="O13">
-        <v>0.10443037974683544</v>
-      </c>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.10426540284360189</v>
+      </c>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+    </row>
+    <row r="14" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="11" t="str">
         <f>CONCATENATE("(",ROUND(L11,3),")")</f>
@@ -1056,7 +1158,7 @@
         <v>(0.094)</v>
       </c>
     </row>
-    <row r="15" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="13">
@@ -1076,8 +1178,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
+    <row r="19" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="20" t="s">
@@ -1087,7 +1189,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="10" t="s">
@@ -1103,7 +1205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="21" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>0</v>
       </c>
@@ -1129,16 +1231,16 @@
         <v>7</v>
       </c>
       <c r="M21">
-        <v>9.0496690936407762E-2</v>
+        <v>0.089525786734281548</v>
       </c>
       <c r="N21">
-        <v>0.14444024088459634</v>
+        <v>0.14131357475231729</v>
       </c>
       <c r="O21">
-        <v>-1.7064098515723318E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+        <v>-0.015359943983193281</v>
+      </c>
+    </row>
+    <row r="22" x14ac:dyDescent="0.35">
       <c r="A22" s="19"/>
       <c r="B22" s="7"/>
       <c r="C22" s="14" t="s">
@@ -1160,16 +1262,16 @@
         <v>7</v>
       </c>
       <c r="M22">
-        <v>0.1158492171094385</v>
+        <v>0.11418028560453146</v>
       </c>
       <c r="N22">
-        <v>0.13230802667771371</v>
+        <v>0.13034246595405036</v>
       </c>
       <c r="O22">
-        <v>0.14484859259458438</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0.14228015768192992</v>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="true" x14ac:dyDescent="0.35">
       <c r="A23" s="19"/>
       <c r="B23" s="6">
         <v>1</v>
@@ -1191,19 +1293,19 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="L23">
-        <v>0.14755341397103675</v>
+        <v>0.14722787537107104</v>
       </c>
       <c r="M23">
-        <v>0.42612564153950472</v>
+        <v>0.42559646095693704</v>
       </c>
       <c r="N23">
-        <v>0.16635650650887082</v>
+        <v>0.16710799701342821</v>
       </c>
       <c r="O23">
-        <v>0.16197325338401591</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+        <v>0.16194911256120592</v>
+      </c>
+    </row>
+    <row r="24" x14ac:dyDescent="0.35">
       <c r="A24" s="19"/>
       <c r="B24" s="7"/>
       <c r="C24" s="14" t="str">
@@ -1223,19 +1325,19 @@
         <v>(0.132)</v>
       </c>
       <c r="L24">
-        <v>0.12702049781867497</v>
+        <v>0.12643272809678782</v>
       </c>
       <c r="M24">
-        <v>0.26378112443849877</v>
+        <v>0.26245937138666531</v>
       </c>
       <c r="N24">
-        <v>0.132118658439972</v>
+        <v>0.13186520124838311</v>
       </c>
       <c r="O24">
-        <v>0.13213925140111349</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+        <v>0.13183019294039244</v>
+      </c>
+    </row>
+    <row r="25" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>1</v>
       </c>
@@ -1258,16 +1360,16 @@
         <v>7</v>
       </c>
       <c r="M25">
-        <v>7.8085477077650969E-2</v>
+        <v>0.07625300289204269</v>
       </c>
       <c r="N25">
-        <v>6.892035878171851E-2</v>
+        <v>0.0689196573063727</v>
       </c>
       <c r="O25">
-        <v>-4.9080578885664986E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>-0.046017102238374068</v>
+      </c>
+    </row>
+    <row r="26" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="13" t="s">
@@ -1289,17 +1391,17 @@
         <v>7</v>
       </c>
       <c r="M26">
-        <v>7.5724436254924921E-2</v>
+        <v>0.073058722289315342</v>
       </c>
       <c r="N26">
-        <v>6.3410448251029705E-2</v>
+        <v>0.063083515145911956</v>
       </c>
       <c r="O26">
-        <v>0.10038106690714045</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.09814611665172078</v>
+      </c>
+    </row>
+    <row r="27" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
+    <row r="29" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="C29" s="16" t="s">
         <v>8</v>
       </c>
@@ -1307,7 +1409,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="C30" s="10" t="s">
         <v>5</v>
       </c>
@@ -1321,7 +1423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="31" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="C31" s="11">
         <f>ROUND(L31,3)</f>
         <v>0.21299999999999999</v>
@@ -1339,37 +1441,37 @@
         <v>0.215</v>
       </c>
       <c r="L31">
-        <v>0.21259198691741618</v>
+        <v>0.21271393643031786</v>
       </c>
       <c r="M31">
-        <v>0.21549295774647886</v>
+        <v>0.2158931082981716</v>
       </c>
       <c r="N31">
-        <v>0.22906403940886699</v>
+        <v>0.22954173486088381</v>
       </c>
       <c r="O31">
-        <v>0.2153846153846154</v>
+        <v>0.21571648690292758</v>
       </c>
       <c r="P31">
-        <v>0.92117487590348524</v>
+        <v>0.91399270862845106</v>
       </c>
       <c r="Q31">
-        <v>0.55591760534177981</v>
+        <v>0.55075851269928044</v>
       </c>
       <c r="R31">
-        <v>0.92817544553152997</v>
+        <v>0.92310759210018689</v>
       </c>
       <c r="S31">
-        <v>0.57907584140368695</v>
+        <v>0.57881908981352537</v>
       </c>
       <c r="T31">
-        <v>0.99689640239812527</v>
+        <v>0.99494292744326185</v>
       </c>
       <c r="U31">
-        <v>0.542154442615294</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+        <v>0.54099317255727974</v>
+      </c>
+    </row>
+    <row r="32" x14ac:dyDescent="0.35">
       <c r="C32" s="11" t="str">
         <f>CONCATENATE("(",ROUND(L32,3),")")</f>
         <v>(0.023)</v>
@@ -1387,19 +1489,25 @@
         <v>(0.021)</v>
       </c>
       <c r="L32">
-        <v>2.2872080473634156E-2</v>
+        <v>0.0230268168640262</v>
       </c>
       <c r="M32">
-        <v>1.8399530077354433E-2</v>
+        <v>0.018397434794207929</v>
       </c>
       <c r="N32">
-        <v>1.6174356828906031E-2</v>
+        <v>0.016362178467322058</v>
       </c>
       <c r="O32">
-        <v>2.0950673136672596E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.020970373568336531</v>
+      </c>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+    </row>
+    <row r="33" x14ac:dyDescent="0.35">
       <c r="C33" s="15">
         <f>L33</f>
         <v>1223</v>
@@ -1417,33 +1525,45 @@
         <v>650</v>
       </c>
       <c r="L33">
-        <v>1223</v>
+        <v>1227</v>
       </c>
       <c r="M33">
-        <v>1420</v>
+        <v>1422</v>
       </c>
       <c r="N33">
-        <v>2436</v>
+        <v>2444</v>
       </c>
       <c r="O33">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+        <v>649</v>
+      </c>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+    </row>
+    <row r="34" x14ac:dyDescent="0.35">
       <c r="L34">
-        <v>0.21347530109966836</v>
+        <v>0.21368861024033436</v>
       </c>
       <c r="M34">
-        <v>0.24786175597835575</v>
+        <v>0.2476489028213166</v>
       </c>
       <c r="N34">
-        <v>0.42520509687554547</v>
+        <v>0.42563566701497735</v>
       </c>
       <c r="O34">
-        <v>0.11345784604643044</v>
-      </c>
-    </row>
-    <row r="35" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.11302681992337164</v>
+      </c>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+    </row>
+    <row r="35" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="C35" s="16" t="s">
         <v>9</v>
       </c>
@@ -1451,7 +1571,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
     </row>
-    <row r="36" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="C36" s="10" t="s">
         <v>5</v>
       </c>
@@ -1465,7 +1585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="37" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="C37" s="11">
         <f>ROUND(L37,3)</f>
         <v>0.115</v>
@@ -1483,37 +1603,37 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="L37">
-        <v>0.11529026982829109</v>
+        <v>0.11409942950285248</v>
       </c>
       <c r="M37">
-        <v>0.11549295774647887</v>
+        <v>0.11533052039381153</v>
       </c>
       <c r="N37">
-        <v>0.10714285714285714</v>
+        <v>0.10761047463175123</v>
       </c>
       <c r="O37">
-        <v>0.10153846153846154</v>
+        <v>0.10169491525423729</v>
       </c>
       <c r="P37">
-        <v>0.99146136885369551</v>
+        <v>0.94779975619234291</v>
       </c>
       <c r="Q37">
-        <v>0.64985571800679431</v>
+        <v>0.71724543306060418</v>
       </c>
       <c r="R37">
-        <v>0.48365525720350733</v>
+        <v>0.52522076097367409</v>
       </c>
       <c r="S37">
-        <v>0.58011910619982388</v>
+        <v>0.60996066477599065</v>
       </c>
       <c r="T37">
-        <v>0.41336221771886927</v>
+        <v>0.42255160564687866</v>
       </c>
       <c r="U37">
-        <v>0.69233383748107036</v>
-      </c>
-    </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.67837635553380848</v>
+      </c>
+    </row>
+    <row r="38" x14ac:dyDescent="0.35">
       <c r="C38" s="11" t="str">
         <f>CONCATENATE("(",ROUND(L38,3),")")</f>
         <v>(0.015)</v>
@@ -1531,19 +1651,25 @@
         <v>(0.013)</v>
       </c>
       <c r="L38">
-        <v>1.5073492993024722E-2</v>
+        <v>0.014950820381161408</v>
       </c>
       <c r="M38">
-        <v>1.150794809496546E-2</v>
+        <v>0.011444443190121258</v>
       </c>
       <c r="N38">
-        <v>9.8004940779611721E-3</v>
+        <v>0.0099355077099445733</v>
       </c>
       <c r="O38">
-        <v>1.2599605142795837E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.012580316315238678</v>
+      </c>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+    </row>
+    <row r="39" x14ac:dyDescent="0.35">
       <c r="C39" s="15">
         <f>L39</f>
         <v>1223</v>
@@ -1561,33 +1687,45 @@
         <v>650</v>
       </c>
       <c r="L39">
-        <v>1223</v>
+        <v>1227</v>
       </c>
       <c r="M39">
-        <v>1420</v>
+        <v>1422</v>
       </c>
       <c r="N39">
-        <v>2436</v>
+        <v>2444</v>
       </c>
       <c r="O39">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.35">
+        <v>649</v>
+      </c>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+    </row>
+    <row r="40" x14ac:dyDescent="0.35">
       <c r="L40">
-        <v>0.21347530109966836</v>
+        <v>0.21368861024033436</v>
       </c>
       <c r="M40">
-        <v>0.24786175597835575</v>
+        <v>0.2476489028213166</v>
       </c>
       <c r="N40">
-        <v>0.42520509687554547</v>
+        <v>0.42563566701497735</v>
       </c>
       <c r="O40">
-        <v>0.11345784604643044</v>
-      </c>
-    </row>
-    <row r="44" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.11302681992337164</v>
+      </c>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+    </row>
+    <row r="44" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A44" s="2"/>
       <c r="B44" s="4"/>
       <c r="C44" s="16" t="s">
@@ -1597,7 +1735,7 @@
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
     </row>
-    <row r="45" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A45" s="3"/>
       <c r="B45" s="5"/>
       <c r="C45" s="10" t="s">
@@ -1613,7 +1751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:47" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="46" ht="15" thickTop="true" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
         <v>0</v>
       </c>
@@ -1637,115 +1775,115 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="L46">
-        <v>6.0362173038229373E-3</v>
+        <v>0.0060120240480961923</v>
       </c>
       <c r="M46">
-        <v>8.7939698492462311E-3</v>
+        <v>0.0088050314465408803</v>
       </c>
       <c r="N46">
-        <v>3.8204393505253103E-3</v>
+        <v>0.0037488284910965324</v>
       </c>
       <c r="O46">
-        <v>3.3112582781456956E-2</v>
+        <v>0.033222591362126248</v>
       </c>
       <c r="P46">
-        <v>4.1322314049586778E-3</v>
+        <v>0.004120879120879121</v>
       </c>
       <c r="Q46">
-        <v>1.6025641025641025E-3</v>
+        <v>0.001594896331738437</v>
       </c>
       <c r="R46">
-        <v>1.4398848092152627E-3</v>
+        <v>0.0014524328249818446</v>
       </c>
       <c r="S46">
-        <v>1.4367816091954023E-2</v>
+        <v>0.014367816091954023</v>
       </c>
       <c r="T46">
-        <v>0.58969992750037326</v>
+        <v>0.58492541949511478</v>
       </c>
       <c r="U46">
-        <v>0.55250971508421043</v>
+        <v>0.54148156927199032</v>
       </c>
       <c r="V46">
-        <v>1.8407068204269555E-2</v>
+        <v>0.018239999803574655</v>
       </c>
       <c r="W46">
-        <v>0.62862683302623001</v>
+        <v>0.63057727488194948</v>
       </c>
       <c r="X46">
-        <v>0.21406078147350102</v>
+        <v>0.21474049885094901</v>
       </c>
       <c r="Y46">
-        <v>0.17229966554926596</v>
+        <v>0.17543204224057382</v>
       </c>
       <c r="Z46">
-        <v>0.24649790188440676</v>
+        <v>0.24395660931920379</v>
       </c>
       <c r="AA46">
-        <v>0.26007222690715609</v>
+        <v>0.25089844541434503</v>
       </c>
       <c r="AB46">
-        <v>3.7829755416234012E-2</v>
+        <v>0.0377391665576036</v>
       </c>
       <c r="AC46">
-        <v>0.35548481337955851</v>
+        <v>0.35301180342678506</v>
       </c>
       <c r="AD46">
-        <v>0.10559072620397023</v>
+        <v>0.10472007726366274</v>
       </c>
       <c r="AE46">
-        <v>7.408212708045564E-2</v>
+        <v>0.074557239524106617</v>
       </c>
       <c r="AF46">
-        <v>0.46089115939483838</v>
+        <v>0.46102687754252369</v>
       </c>
       <c r="AG46">
-        <v>9.0264384448070067E-3</v>
+        <v>0.008874761218385702</v>
       </c>
       <c r="AH46">
-        <v>0.93152462716313278</v>
+        <v>0.91774241272672907</v>
       </c>
       <c r="AI46">
-        <v>0.36720008178973473</v>
+        <v>0.37466786909724459</v>
       </c>
       <c r="AJ46">
-        <v>0.27444268091051138</v>
+        <v>0.28535800766864183</v>
       </c>
       <c r="AK46">
-        <v>0.11877671030537655</v>
+        <v>0.11438698270372287</v>
       </c>
       <c r="AL46">
-        <v>1.1481977701865318E-2</v>
+        <v>0.011423817357448926</v>
       </c>
       <c r="AM46">
-        <v>4.8019108587179253E-3</v>
+        <v>0.00480427230210581</v>
       </c>
       <c r="AN46">
-        <v>4.4813094464451761E-3</v>
+        <v>0.0045169643579712031</v>
       </c>
       <c r="AO46">
-        <v>9.829865334150048E-2</v>
+        <v>0.096044356938113834</v>
       </c>
       <c r="AP46">
-        <v>0.46430199723748322</v>
+        <v>0.46363221479392958</v>
       </c>
       <c r="AQ46">
-        <v>0.40773426203941454</v>
+        <v>0.4112414079134078</v>
       </c>
       <c r="AR46">
-        <v>0.15189501258061022</v>
+        <v>0.15035691361758227</v>
       </c>
       <c r="AS46">
-        <v>0.9300658344299777</v>
+        <v>0.93870889851680639</v>
       </c>
       <c r="AT46">
-        <v>5.4480493222876347E-2</v>
+        <v>0.053669584476110435</v>
       </c>
       <c r="AU46">
-        <v>4.8449546729351228E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.048129603725297572</v>
+      </c>
+    </row>
+    <row r="47" x14ac:dyDescent="0.35">
       <c r="A47" s="18"/>
       <c r="B47" s="6"/>
       <c r="C47" s="11" t="str">
@@ -1765,31 +1903,59 @@
         <v>(0.011)</v>
       </c>
       <c r="L47">
-        <v>3.2097112650795938E-3</v>
+        <v>0.003204260970733308</v>
       </c>
       <c r="M47">
-        <v>3.9863207725839176E-3</v>
+        <v>0.0039901551507228209</v>
       </c>
       <c r="N47">
-        <v>1.912172940715021E-3</v>
+        <v>0.0018751346051772493</v>
       </c>
       <c r="O47">
-        <v>1.0940016107615524E-2</v>
+        <v>0.010982889954204976</v>
       </c>
       <c r="P47">
-        <v>3.0920931358299391E-3</v>
+        <v>0.0030842143682750637</v>
       </c>
       <c r="Q47">
-        <v>1.547585312409367E-3</v>
+        <v>0.0015405073278882606</v>
       </c>
       <c r="R47">
-        <v>1.0274815285485808E-3</v>
+        <v>0.0010364111528403019</v>
       </c>
       <c r="S47">
-        <v>6.4219294058349254E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.35">
+        <v>0.00640459405855426</v>
+      </c>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+      <c r="Y47"/>
+      <c r="Z47"/>
+      <c r="AA47"/>
+      <c r="AB47"/>
+      <c r="AC47"/>
+      <c r="AD47"/>
+      <c r="AE47"/>
+      <c r="AF47"/>
+      <c r="AG47"/>
+      <c r="AH47"/>
+      <c r="AI47"/>
+      <c r="AJ47"/>
+      <c r="AK47"/>
+      <c r="AL47"/>
+      <c r="AM47"/>
+      <c r="AN47"/>
+      <c r="AO47"/>
+      <c r="AP47"/>
+      <c r="AQ47"/>
+      <c r="AR47"/>
+      <c r="AS47"/>
+      <c r="AT47"/>
+      <c r="AU47"/>
+    </row>
+    <row r="48" x14ac:dyDescent="0.35">
       <c r="A48" s="18"/>
       <c r="B48" s="7"/>
       <c r="C48" s="12">
@@ -1809,31 +1975,59 @@
         <v>534</v>
       </c>
       <c r="L48">
-        <v>800</v>
+        <v>818</v>
       </c>
       <c r="M48">
-        <v>1504</v>
+        <v>1523</v>
       </c>
       <c r="N48">
-        <v>1763</v>
+        <v>1803</v>
       </c>
       <c r="O48">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="P48">
-        <v>1122</v>
+        <v>1115</v>
       </c>
       <c r="Q48">
-        <v>946</v>
+        <v>938</v>
       </c>
       <c r="R48">
-        <v>2082</v>
+        <v>2069</v>
       </c>
       <c r="S48">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+        <v>480</v>
+      </c>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+      <c r="X48"/>
+      <c r="Y48"/>
+      <c r="Z48"/>
+      <c r="AA48"/>
+      <c r="AB48"/>
+      <c r="AC48"/>
+      <c r="AD48"/>
+      <c r="AE48"/>
+      <c r="AF48"/>
+      <c r="AG48"/>
+      <c r="AH48"/>
+      <c r="AI48"/>
+      <c r="AJ48"/>
+      <c r="AK48"/>
+      <c r="AL48"/>
+      <c r="AM48"/>
+      <c r="AN48"/>
+      <c r="AO48"/>
+      <c r="AP48"/>
+      <c r="AQ48"/>
+      <c r="AR48"/>
+      <c r="AS48"/>
+      <c r="AT48"/>
+      <c r="AU48"/>
+    </row>
+    <row r="49" x14ac:dyDescent="0.35">
       <c r="A49" s="18"/>
       <c r="B49" s="6">
         <v>1</v>
@@ -1855,31 +2049,59 @@
         <v>1.4E-2</v>
       </c>
       <c r="L49">
-        <v>8.6673889490790898E-2</v>
+        <v>0.088165552920888124</v>
       </c>
       <c r="M49">
-        <v>0.1629469122426869</v>
+        <v>0.16415175684414746</v>
       </c>
       <c r="N49">
-        <v>0.19100758396533044</v>
+        <v>0.19433067471437809</v>
       </c>
       <c r="O49">
-        <v>5.7854821235102924E-2</v>
+        <v>0.057339943953438242</v>
       </c>
       <c r="P49">
-        <v>0.12156013001083424</v>
+        <v>0.12017676223323992</v>
       </c>
       <c r="Q49">
-        <v>0.10249187432286024</v>
+        <v>0.10109937486527269</v>
       </c>
       <c r="R49">
-        <v>0.22556879739978331</v>
+        <v>0.22300064669109723</v>
       </c>
       <c r="S49">
-        <v>5.1895991332611052E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+        <v>0.051735287777538261</v>
+      </c>
+      <c r="T49"/>
+      <c r="U49"/>
+      <c r="V49"/>
+      <c r="W49"/>
+      <c r="X49"/>
+      <c r="Y49"/>
+      <c r="Z49"/>
+      <c r="AA49"/>
+      <c r="AB49"/>
+      <c r="AC49"/>
+      <c r="AD49"/>
+      <c r="AE49"/>
+      <c r="AF49"/>
+      <c r="AG49"/>
+      <c r="AH49"/>
+      <c r="AI49"/>
+      <c r="AJ49"/>
+      <c r="AK49"/>
+      <c r="AL49"/>
+      <c r="AM49"/>
+      <c r="AN49"/>
+      <c r="AO49"/>
+      <c r="AP49"/>
+      <c r="AQ49"/>
+      <c r="AR49"/>
+      <c r="AS49"/>
+      <c r="AT49"/>
+      <c r="AU49"/>
+    </row>
+    <row r="50" x14ac:dyDescent="0.35">
       <c r="A50" s="18"/>
       <c r="B50" s="6"/>
       <c r="C50" s="11" t="str">
@@ -1899,7 +2121,7 @@
         <v>(0.006)</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="51" x14ac:dyDescent="0.35">
       <c r="A51" s="18"/>
       <c r="B51" s="7"/>
       <c r="C51" s="12">
@@ -1919,37 +2141,37 @@
         <v>479</v>
       </c>
       <c r="L51">
-        <v>4.9059689288634507E-3</v>
+        <v>0.0048899755501222494</v>
       </c>
       <c r="M51">
-        <v>5.6338028169014088E-3</v>
+        <v>0.0056258790436005627</v>
       </c>
       <c r="N51">
-        <v>2.4630541871921183E-3</v>
+        <v>0.0024549918166939444</v>
       </c>
       <c r="O51">
-        <v>2.3076923076923078E-2</v>
+        <v>0.023112480739599383</v>
       </c>
       <c r="P51">
-        <v>0.82852764560199688</v>
+        <v>0.82625887998529457</v>
       </c>
       <c r="Q51">
-        <v>0.36171005565460346</v>
+        <v>0.36176927289542393</v>
       </c>
       <c r="R51">
-        <v>1.3382051452367592E-2</v>
+        <v>0.013286950018130404</v>
       </c>
       <c r="S51">
-        <v>0.20130660961618221</v>
+        <v>0.20048084102508687</v>
       </c>
       <c r="T51">
-        <v>1.6472860420285621E-2</v>
+        <v>0.016425144992040699</v>
       </c>
       <c r="U51">
-        <v>3.4068444991565811E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+        <v>0.0034111968878727294</v>
+      </c>
+    </row>
+    <row r="52" x14ac:dyDescent="0.35">
       <c r="B52" s="6" t="s">
         <v>1</v>
       </c>
@@ -1970,19 +2192,25 @@
         <v>2.3E-2</v>
       </c>
       <c r="L52">
-        <v>2.4848151172649161E-3</v>
+        <v>0.0024772157959131475</v>
       </c>
       <c r="M52">
-        <v>2.2685807958589595E-3</v>
+        <v>0.0022652903879362952</v>
       </c>
       <c r="N52">
-        <v>1.011381433704327E-3</v>
+        <v>0.0010078306826754473</v>
       </c>
       <c r="O52">
-        <v>6.8577616757890571E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+        <v>0.0068743749146813679</v>
+      </c>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+    </row>
+    <row r="53" x14ac:dyDescent="0.35">
       <c r="B53" s="6"/>
       <c r="C53" s="11" t="str">
         <f>CONCATENATE("(",ROUND(L52,3),")")</f>
@@ -2001,19 +2229,25 @@
         <v>(0.007)</v>
       </c>
       <c r="L53">
-        <v>1922</v>
+        <v>1933</v>
       </c>
       <c r="M53">
-        <v>2450</v>
+        <v>2461</v>
       </c>
       <c r="N53">
-        <v>3845</v>
+        <v>3872</v>
       </c>
       <c r="O53">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>1012</v>
+      </c>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="S53"/>
+      <c r="T53"/>
+      <c r="U53"/>
+    </row>
+    <row r="54" ht="15" thickBot="true" x14ac:dyDescent="0.4">
       <c r="A54" s="8"/>
       <c r="B54" s="9"/>
       <c r="C54" s="13">
@@ -2033,19 +2267,25 @@
         <v>1013</v>
       </c>
       <c r="L54">
-        <v>0.20823401950162512</v>
+        <v>0.20834231515412804</v>
       </c>
       <c r="M54">
-        <v>0.26543878656554715</v>
+        <v>0.26525113170942011</v>
       </c>
       <c r="N54">
-        <v>0.41657638136511377</v>
+        <v>0.4173313214054753</v>
       </c>
       <c r="O54">
-        <v>0.10975081256771398</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>0.10907523173097651</v>
+      </c>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+      <c r="S54"/>
+      <c r="T54"/>
+      <c r="U54"/>
+    </row>
+    <row r="55" ht="15" thickTop="true" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="C44:F44"/>

</xml_diff>